<commit_message>
single row WriteToExcel in Library and UserManagement
</commit_message>
<xml_diff>
--- a/libraryBooks.xlsx
+++ b/libraryBooks.xlsx
@@ -484,12 +484,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12, 9000]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 156.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 156 cancelled their reservation', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.', 'User 9000 cancelled their reservation', 'User 12 cancelled their reservation', 'Resereved by user 12.', 'Resereved by user 9000.']</t>
         </is>
       </c>
     </row>
@@ -512,12 +512,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[156]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.', 'User 156 cancelled their reservation', 'Resereved by user 156.']</t>
         </is>
       </c>
     </row>

</xml_diff>